<commit_message>
Fixed pair retrieval, and displayed counts
</commit_message>
<xml_diff>
--- a/extras/sample-form/Detect clicked link sample form.xlsx
+++ b/extras/sample-form/Detect clicked link sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/detect-clicked-link/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17955F1-7413-934C-AAFD-83CD29D403C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C3A66-944A-C94C-8E66-B820FAC47AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31700" yWindow="-1680" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36140" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="407">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2640,15 +2640,9 @@
     <t>link_data</t>
   </si>
   <si>
-    <t>item-at('|', ${example1_metadata}, ${link_num})</t>
-  </si>
-  <si>
     <t>link_url</t>
   </si>
   <si>
-    <t>link_clicked</t>
-  </si>
-  <si>
     <t>selected-at(${link_data}, 0)</t>
   </si>
   <si>
@@ -2658,15 +2652,9 @@
     <t>all_counts</t>
   </si>
   <si>
-    <t>join(' ', ${link_clicked})</t>
-  </si>
-  <si>
     <t>not_clicked</t>
   </si>
   <si>
-    <t>Please go back and open all of the links.</t>
-  </si>
-  <si>
     <t>selected(${all_counts}, '0')</t>
   </si>
   <si>
@@ -2674,9 +2662,6 @@
   </si>
   <si>
     <t>complete</t>
-  </si>
-  <si>
-    <t>Thank you for clicking on those links!</t>
   </si>
   <si>
     <t>custom-detect-clicked-link</t>
@@ -2684,6 +2669,56 @@
   <si>
     <t>&lt;p&gt;To learn more about the Data Explorer, check out our documentation on &lt;a href="https://docs.surveycto.com/04-monitoring-and-management/01-the-basics/03a.using-data-explorer.html" target="_blank"&gt;using the Data Explorer to monitor incoming data&lt;/a&gt;. To learn more about the review and corrections workflow, check out our documentation on &lt;a href="https://docs.surveycto.com/04-monitoring-and-management/01-the-basics/04.reviewing-and-correcting.html" target="_blank"&gt;reviewing and correcting incoming data&lt;/a&gt;.&lt;p&gt;
 &lt;p&gt;Did you click on both of those links?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>click_count</t>
+  </si>
+  <si>
+    <t>join(' ', ${click_count})</t>
+  </si>
+  <si>
+    <t>all_click_count</t>
+  </si>
+  <si>
+    <t>Please go back and open all of the links.
+${all_click_count}</t>
+  </si>
+  <si>
+    <t>Thank you for clicking on those links!
+${all_click_count}</t>
+  </si>
+  <si>
+    <t>click_disp</t>
+  </si>
+  <si>
+    <t>concat('Link ', ${link_num}, ': ', ${click_count})</t>
+  </si>
+  <si>
+    <t>Link number</t>
+  </si>
+  <si>
+    <t>Retrieve data pair</t>
+  </si>
+  <si>
+    <t>URL of link to be clicked</t>
+  </si>
+  <si>
+    <t>Number of times link has been clicked</t>
+  </si>
+  <si>
+    <t>All click counts, used to determine if any have been clicked 0 times</t>
+  </si>
+  <si>
+    <t>Optional: Used to display the click counts</t>
+  </si>
+  <si>
+    <t>Optional: Holds all click counts for display purposes</t>
+  </si>
+  <si>
+    <t>join(linebreak(), ${click_disp})</t>
+  </si>
+  <si>
+    <t>item-at('|', ${example1_metadata}, ${link_num} - 1)</t>
   </si>
 </sst>
 </file>
@@ -4833,13 +4868,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5043,10 +5078,10 @@
         <v>371</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -5087,95 +5122,138 @@
         <v>378</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>379</v>
       </c>
+      <c r="C16" s="10" t="s">
+        <v>398</v>
+      </c>
       <c r="N16" s="9" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>380</v>
       </c>
+      <c r="C17" s="10" t="s">
+        <v>399</v>
+      </c>
       <c r="N17" s="9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="N18" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="N18" s="9" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="N19" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>376</v>
+        <v>396</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>391</v>
+        <v>402</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>393</v>
+      <c r="B24" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -5477,7 +5555,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2107231859</v>
+        <v>2108021143</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>370</v>

</xml_diff>